<commit_message>
signature_2 is added in all keolis forms except weekly inspection
</commit_message>
<xml_diff>
--- a/app/config/tables/USTMonthlyInspectionForSPCCP/forms/USTMonthlyInspectionForSPCCP/USTMonthlyInspectionForSPCCP.xlsx
+++ b/app/config/tables/USTMonthlyInspectionForSPCCP/forms/USTMonthlyInspectionForSPCCP/USTMonthlyInspectionForSPCCP.xlsx
@@ -9,10 +9,11 @@
     <sheet state="visible" name="notes_section" sheetId="4" r:id="rId6"/>
     <sheet state="visible" name="image_section" sheetId="5" r:id="rId7"/>
     <sheet state="visible" name="signature_section" sheetId="6" r:id="rId8"/>
-    <sheet state="visible" name="choices" sheetId="7" r:id="rId9"/>
-    <sheet state="visible" name="queries" sheetId="8" r:id="rId10"/>
-    <sheet state="visible" name="settings" sheetId="9" r:id="rId11"/>
-    <sheet state="visible" name="calculates" sheetId="10" r:id="rId12"/>
+    <sheet state="visible" name="signature_2_section" sheetId="7" r:id="rId9"/>
+    <sheet state="visible" name="choices" sheetId="8" r:id="rId10"/>
+    <sheet state="visible" name="queries" sheetId="9" r:id="rId11"/>
+    <sheet state="visible" name="settings" sheetId="10" r:id="rId12"/>
+    <sheet state="visible" name="calculates" sheetId="11" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -38,12 +39,12 @@
       <color rgb="FF444444"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <sz val="11.0"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color rgb="FF444444"/>
       <name val="'Trebuchet MS'"/>
@@ -89,70 +90,70 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
     <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>

</xml_diff>

<commit_message>
z1_next_photo_index field added in all forms
</commit_message>
<xml_diff>
--- a/app/config/tables/USTMonthlyInspectionForSPCCP/forms/USTMonthlyInspectionForSPCCP/USTMonthlyInspectionForSPCCP.xlsx
+++ b/app/config/tables/USTMonthlyInspectionForSPCCP/forms/USTMonthlyInspectionForSPCCP/USTMonthlyInspectionForSPCCP.xlsx
@@ -29,25 +29,25 @@
       <name val="Arial"/>
     </font>
     <font>
-      <name val="Arial"/>
-    </font>
-    <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <color rgb="FF444444"/>
-      <name val="Arial"/>
-    </font>
-    <font/>
+      <name val="Arial"/>
+    </font>
     <font>
       <sz val="11.0"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <color rgb="FF444444"/>
       <name val="'Trebuchet MS'"/>
+    </font>
+    <font>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
     </font>
     <font>
       <color rgb="FF444444"/>
@@ -100,23 +100,28 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -125,58 +130,53 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -185,42 +185,42 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
     </xf>
   </cellXfs>
   <cellStyles count="1">

</xml_diff>